<commit_message>
Scripting DPLKINV061-001 until DPLKINV065-001 (Setup Emiten)
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV061-001 - Setup Emiten Investasi - General Tambah Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV061-001 - Setup Emiten Investasi - General Tambah Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F29AC9D-8CFD-4917-90A5-F54BA16C6899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C5351B-DDDA-454D-B26D-A57A5DB9676B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -197,6 +197,21 @@
   </si>
   <si>
     <t>Analisis Investasi</t>
+  </si>
+  <si>
+    <t>0123456789</t>
+  </si>
+  <si>
+    <t>1 : Lanjutkan ke Verifikasi</t>
+  </si>
+  <si>
+    <t>DATA UNTUK DIVERIFIKASI</t>
+  </si>
+  <si>
+    <t>Tambah Dapat dilakukan dengan baik</t>
+  </si>
+  <si>
+    <t>Sucorinvest Adidaya, PT</t>
   </si>
   <si>
     <t>Username : 31246;
@@ -205,7 +220,7 @@
 Kode Emiten : -;
 Group Emiten : BCA Group;
 Jenis Emiten : Swasta;
-Nama Emiten : Tester;
+Nama Emiten : Sucorinvest Adidaya, PT;
 Ticker : Test;
 Keterangan : INV.SET.013;
 Sektor : 4 - Keuangan;
@@ -227,18 +242,6 @@
 Default : Ya;
 Status Register : 1 : Lanjutkan ke Verifikasi;
 Keterangan Register : DATA UNTUK DIVERIFIKASI</t>
-  </si>
-  <si>
-    <t>0123456789</t>
-  </si>
-  <si>
-    <t>1 : Lanjutkan ke Verifikasi</t>
-  </si>
-  <si>
-    <t>DATA UNTUK DIVERIFIKASI</t>
-  </si>
-  <si>
-    <t>Tambah Dapat dilakukan dengan baik</t>
   </si>
 </sst>
 </file>
@@ -646,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AK1" sqref="AK1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,10 +822,10 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G2" s="4">
         <v>31246</v>
@@ -849,8 +852,8 @@
       <c r="O2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>43</v>
+      <c r="P2" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>44</v>
@@ -883,7 +886,7 @@
         <v>123456789</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB2" s="1">
         <v>99999999</v>
@@ -892,10 +895,10 @@
         <v>51</v>
       </c>
       <c r="AD2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE2" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="AE2" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>52</v>

</xml_diff>